<commit_message>
Updated Gmail username and password
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
-  <si>
-    <t>Gmail</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Facebook</t>
   </si>
@@ -51,13 +48,10 @@
     <t>DEF</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>tr</t>
+    <t>Gmail 1</t>
+  </si>
+  <si>
+    <t>Gmail 2</t>
   </si>
 </sst>
 </file>
@@ -387,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -410,33 +404,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>9431512849</v>
@@ -444,25 +432,31 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>